<commit_message>
Quiz Done and Sentences Done, UI Changed - Need Musa to Change Controllers to Make Further Changes
</commit_message>
<xml_diff>
--- a/public/templates/practice_sentences_template.xlsx
+++ b/public/templates/practice_sentences_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basit\Dropbox\My PC (LAPTOP-L7PDQOB1)\Downloads\JMR\ADMIN\JMR-Admin\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC130153-BC17-4AB4-AF2B-617254619186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651F6FBB-D388-4B15-B996-71BAA35CAEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6470C26C-2F8F-4562-903F-F3CCA5958D17}"/>
   </bookViews>
@@ -36,20 +36,388 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>title</t>
   </si>
   <si>
     <t>modal_sentence</t>
+  </si>
+  <si>
+    <t>Ability</t>
+  </si>
+  <si>
+    <t>Past Ability</t>
+  </si>
+  <si>
+    <t>Can</t>
+  </si>
+  <si>
+    <t>I can speak three languages fluently.</t>
+  </si>
+  <si>
+    <t>She can lift the heavy box.</t>
+  </si>
+  <si>
+    <t>You can park your car on the street.</t>
+  </si>
+  <si>
+    <t>He can fix broken electronics.</t>
+  </si>
+  <si>
+    <t>We can meet at 4 PM tomorrow.</t>
+  </si>
+  <si>
+    <t>They can finish the project early.</t>
+  </si>
+  <si>
+    <t>Can you hear that music playing?</t>
+  </si>
+  <si>
+    <t>The students can use their notes.</t>
+  </si>
+  <si>
+    <t>I can recognize her voice easily.</t>
+  </si>
+  <si>
+    <t>Our team can handle the challenge.</t>
+  </si>
+  <si>
+    <t>Could</t>
+  </si>
+  <si>
+    <t>When I was young, I could run very fast.</t>
+  </si>
+  <si>
+    <t>He could play the piano before he was ten.</t>
+  </si>
+  <si>
+    <t>I could help you with your homework.</t>
+  </si>
+  <si>
+    <t>Could I borrow your pen, please?</t>
+  </si>
+  <si>
+    <t>It could rain later this afternoon.</t>
+  </si>
+  <si>
+    <t>The old machine could cut metal easily.</t>
+  </si>
+  <si>
+    <t>She could have been a professional artist.</t>
+  </si>
+  <si>
+    <t>We could try calling him one more time.</t>
+  </si>
+  <si>
+    <t>I could see the ocean from my window.</t>
+  </si>
+  <si>
+    <t>They could not attend the meeting yesterday.</t>
+  </si>
+  <si>
+    <t>Possibility</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>The flight may be delayed due to fog.</t>
+  </si>
+  <si>
+    <t>You may use my laptop for your presentation.</t>
+  </si>
+  <si>
+    <t>May I take a look at the data sheet?</t>
+  </si>
+  <si>
+    <t>She may arrive any minute now.</t>
+  </si>
+  <si>
+    <t>The report may contain a few minor errors.</t>
+  </si>
+  <si>
+    <t>We may go to the cinema this weekend.</t>
+  </si>
+  <si>
+    <t>This method may be more efficient than the last one.</t>
+  </si>
+  <si>
+    <t>You may leave the class early today.</t>
+  </si>
+  <si>
+    <t>He may not agree with the new policy.</t>
+  </si>
+  <si>
+    <t>That solution may cause a new set of problems.</t>
+  </si>
+  <si>
+    <t>Weak Possibility</t>
+  </si>
+  <si>
+    <t>Might</t>
+  </si>
+  <si>
+    <t>I might accept the job offer next week.</t>
+  </si>
+  <si>
+    <t>He might not be at home right now.</t>
+  </si>
+  <si>
+    <t>The concert might be sold out already.</t>
+  </si>
+  <si>
+    <t>We might catch the early train if we hurry.</t>
+  </si>
+  <si>
+    <t>You might find the answer in the appendix.</t>
+  </si>
+  <si>
+    <t>They might be meeting in the conference room.</t>
+  </si>
+  <si>
+    <t>This decision might affect our long-term goals.</t>
+  </si>
+  <si>
+    <t>She might have forgotten her keys inside.</t>
+  </si>
+  <si>
+    <t>It might snow in the mountains tonight.</t>
+  </si>
+  <si>
+    <t>We might as well start without him.</t>
+  </si>
+  <si>
+    <t>Strong Obligation</t>
+  </si>
+  <si>
+    <t>Must</t>
+  </si>
+  <si>
+    <t>You must wear a seatbelt at all times.</t>
+  </si>
+  <si>
+    <t>Students must submit the assignment by Friday.</t>
+  </si>
+  <si>
+    <t>We must check the data for accuracy.</t>
+  </si>
+  <si>
+    <t>The manager must approve all expenses.</t>
+  </si>
+  <si>
+    <t>This password must contain a special character.</t>
+  </si>
+  <si>
+    <t>You must not talk during the exam.</t>
+  </si>
+  <si>
+    <t>He must be exhausted after that long trip.</t>
+  </si>
+  <si>
+    <t>I must call my mother tonight.</t>
+  </si>
+  <si>
+    <t>They must finish the construction on schedule.</t>
+  </si>
+  <si>
+    <t>The document must be notarized immediately.</t>
+  </si>
+  <si>
+    <t>Advice/Necessity</t>
+  </si>
+  <si>
+    <t>Should</t>
+  </si>
+  <si>
+    <t>You should try to get more sleep.</t>
+  </si>
+  <si>
+    <t>We should invest in better software.</t>
+  </si>
+  <si>
+    <t>I should apologize for my mistake.</t>
+  </si>
+  <si>
+    <t>The package should arrive by tomorrow morning.</t>
+  </si>
+  <si>
+    <t>Should I send the email now or wait?</t>
+  </si>
+  <si>
+    <t>She should review the safety procedures.</t>
+  </si>
+  <si>
+    <t>They should know the rules by now.</t>
+  </si>
+  <si>
+    <t>He should have called a taxi instead.</t>
+  </si>
+  <si>
+    <t>This painting should be worth a lot of money.</t>
+  </si>
+  <si>
+    <t>You should not rely on public Wi-Fi.</t>
+  </si>
+  <si>
+    <t>Request/Intention</t>
+  </si>
+  <si>
+    <t>Will</t>
+  </si>
+  <si>
+    <t>I will definitely attend the ceremony.</t>
+  </si>
+  <si>
+    <t>Will you please close the door quietly?</t>
+  </si>
+  <si>
+    <t>The software will update overnight.</t>
+  </si>
+  <si>
+    <t>He will be our project lead for the next quarter.</t>
+  </si>
+  <si>
+    <t>We will not tolerate any misconduct here.</t>
+  </si>
+  <si>
+    <t>Will the presentation start on time?</t>
+  </si>
+  <si>
+    <t>The weather forecast says it will be sunny.</t>
+  </si>
+  <si>
+    <t>I will send the contract over right away.</t>
+  </si>
+  <si>
+    <t>She will take care of the arrangement.</t>
+  </si>
+  <si>
+    <t>Will you accept this job offer?</t>
+  </si>
+  <si>
+    <t>Polite Request/Habit</t>
+  </si>
+  <si>
+    <t>Would</t>
+  </si>
+  <si>
+    <t>Would you mind helping me with this task?</t>
+  </si>
+  <si>
+    <t>I would appreciate your feedback on this design.</t>
+  </si>
+  <si>
+    <t>He would often skip his morning coffee.</t>
+  </si>
+  <si>
+    <t>Would you like a glass of water?</t>
+  </si>
+  <si>
+    <t>If I had time, I would travel the world.</t>
+  </si>
+  <si>
+    <t>The machine would always break down on Mondays.</t>
+  </si>
+  <si>
+    <t>Would you call back later this afternoon?</t>
+  </si>
+  <si>
+    <t>She would never tell anyone her secrets.</t>
+  </si>
+  <si>
+    <t>That would be an excellent idea.</t>
+  </si>
+  <si>
+    <t>We would always meet here after school.</t>
+  </si>
+  <si>
+    <t>Formal Obligation/Offer</t>
+  </si>
+  <si>
+    <t>Shall</t>
+  </si>
+  <si>
+    <t>Shall we begin the meeting now?</t>
+  </si>
+  <si>
+    <t>You shall receive your final grade by email.</t>
+  </si>
+  <si>
+    <t>I shall abide by the terms of the agreement.</t>
+  </si>
+  <si>
+    <t>Shall I bring the documents with me?</t>
+  </si>
+  <si>
+    <t>We shall overcome these logistical issues.</t>
+  </si>
+  <si>
+    <t>They shall be informed of the outcome promptly.</t>
+  </si>
+  <si>
+    <t>Shall we order some coffee for the guests?</t>
+  </si>
+  <si>
+    <t>The committee shall vote on the proposal next month.</t>
+  </si>
+  <si>
+    <t>You shall not pass this gate without permission.</t>
+  </si>
+  <si>
+    <t>The company shall provide all necessary training.</t>
+  </si>
+  <si>
+    <t>Soft Obligation</t>
+  </si>
+  <si>
+    <t>Ought to</t>
+  </si>
+  <si>
+    <t>You ought to see a doctor about that cough.</t>
+  </si>
+  <si>
+    <t>We ought to save money for our retirement.</t>
+  </si>
+  <si>
+    <t>They ought to check the expiration date on the milk.</t>
+  </si>
+  <si>
+    <t>He ought to apologize for his rude comments.</t>
+  </si>
+  <si>
+    <t>I ought to start packing for the trip tonight.</t>
+  </si>
+  <si>
+    <t>The car ought to be serviced regularly.</t>
+  </si>
+  <si>
+    <t>She ought to be more careful with sensitive data.</t>
+  </si>
+  <si>
+    <t>You ought to have told me the truth earlier.</t>
+  </si>
+  <si>
+    <t>The government ought to address climate change.</t>
+  </si>
+  <si>
+    <t>You ought to respect your elders.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -77,8 +445,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,11 +782,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846B2CCE-383E-41A8-BB6C-6BBC24D061D8}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,7 +832,388 @@
         <v>10</v>
       </c>
     </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G8" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" t="s">
+        <v>82</v>
+      </c>
+      <c r="J8" t="s">
+        <v>83</v>
+      </c>
+      <c r="K8" t="s">
+        <v>84</v>
+      </c>
+      <c r="L8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9" t="s">
+        <v>94</v>
+      </c>
+      <c r="J9" t="s">
+        <v>95</v>
+      </c>
+      <c r="K9" t="s">
+        <v>96</v>
+      </c>
+      <c r="L9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
+        <v>99</v>
+      </c>
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" t="s">
+        <v>103</v>
+      </c>
+      <c r="G10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10" t="s">
+        <v>106</v>
+      </c>
+      <c r="J10" t="s">
+        <v>107</v>
+      </c>
+      <c r="K10" t="s">
+        <v>108</v>
+      </c>
+      <c r="L10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D11" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H11" t="s">
+        <v>117</v>
+      </c>
+      <c r="I11" t="s">
+        <v>118</v>
+      </c>
+      <c r="J11" t="s">
+        <v>119</v>
+      </c>
+      <c r="K11" t="s">
+        <v>120</v>
+      </c>
+      <c r="L11" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>